<commit_message>
Update most parts of the code
</commit_message>
<xml_diff>
--- a/Feature-Analysis/Resize Feature/s_01_left.xlsx
+++ b/Feature-Analysis/Resize Feature/s_01_left.xlsx
@@ -1687,7 +1687,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="0">
-        <v>737791.52777777775</v>
+        <v>738157.52777777775</v>
       </c>
       <c r="C2" s="0">
         <v>0</v>
@@ -2382,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="0">
-        <v>737791.52851851855</v>
+        <v>738157.52851851855</v>
       </c>
       <c r="C3" s="0">
         <v>64.000004902482033</v>
@@ -3077,7 +3077,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="0">
-        <v>737791.52885416662</v>
+        <v>738157.52885416662</v>
       </c>
       <c r="C4" s="0">
         <v>92.999998480081558</v>
@@ -3772,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="0">
-        <v>737791.52921296295</v>
+        <v>738157.52921296295</v>
       </c>
       <c r="C5" s="0">
         <v>124.00000132620335</v>
@@ -4467,7 +4467,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0">
-        <v>737791.52956018515</v>
+        <v>738157.52956018515</v>
       </c>
       <c r="C6" s="0">
         <v>153.999999538064</v>
@@ -5162,7 +5162,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="0">
-        <v>737791.52990740736</v>
+        <v>738157.52990740736</v>
       </c>
       <c r="C7" s="0">
         <v>183.99999774992466</v>
@@ -5857,7 +5857,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="0">
-        <v>737791.53021990741</v>
+        <v>738157.53021990741</v>
       </c>
       <c r="C8" s="0">
         <v>211.00000217556953</v>
@@ -6552,7 +6552,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="0">
-        <v>737791.53057870374</v>
+        <v>738157.53057870374</v>
       </c>
       <c r="C9" s="0">
         <v>242.00000502169132</v>
@@ -7247,7 +7247,7 @@
         <v>1</v>
       </c>
       <c r="B10" s="0">
-        <v>737791.53094907408</v>
+        <v>738157.53094907408</v>
       </c>
       <c r="C10" s="0">
         <v>274.00000244379044</v>
@@ -7942,7 +7942,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="0">
-        <v>737791.53129629628</v>
+        <v>738157.53129629628</v>
       </c>
       <c r="C11" s="0">
         <v>304.00000065565109</v>
@@ -8637,7 +8637,7 @@
         <v>1</v>
       </c>
       <c r="B12" s="0">
-        <v>737791.53164351848</v>
+        <v>738157.53164351848</v>
       </c>
       <c r="C12" s="0">
         <v>333.99999886751175</v>
@@ -9332,7 +9332,7 @@
         <v>1</v>
       </c>
       <c r="B13" s="0">
-        <v>737791.53199074068</v>
+        <v>738157.53199074068</v>
       </c>
       <c r="C13" s="0">
         <v>363.99999707937241</v>
@@ -10027,7 +10027,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="0">
-        <v>737791.53238425928</v>
+        <v>738157.53238425928</v>
       </c>
       <c r="C14" s="0">
         <v>398.00000376999378</v>
@@ -10722,7 +10722,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="0">
-        <v>737791.53270833334</v>
+        <v>738157.53270833334</v>
       </c>
       <c r="C15" s="0">
         <v>426.00000277161598</v>
@@ -11417,7 +11417,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="0">
-        <v>737791.53302083327</v>
+        <v>738157.53302083327</v>
       </c>
       <c r="C16" s="0">
         <v>452.99999713897705</v>
@@ -12112,7 +12112,7 @@
         <v>1</v>
       </c>
       <c r="B17" s="0">
-        <v>737791.53339120373</v>
+        <v>738157.53339120373</v>
       </c>
       <c r="C17" s="0">
         <v>485.00000461935997</v>
@@ -12807,7 +12807,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="0">
-        <v>737791.53407407412</v>
+        <v>738157.53407407412</v>
       </c>
       <c r="C18" s="0">
         <v>544.00000646710396</v>
@@ -13502,7 +13502,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="0">
-        <v>737791.53442129632</v>
+        <v>738157.53442129632</v>
       </c>
       <c r="C19" s="0">
         <v>574.00000467896461</v>
@@ -14197,7 +14197,7 @@
         <v>1</v>
       </c>
       <c r="B20" s="0">
-        <v>737791.5347569444</v>
+        <v>738157.5347569444</v>
       </c>
       <c r="C20" s="0">
         <v>602.99999825656414</v>
@@ -14892,7 +14892,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="0">
-        <v>737791.53510416672</v>
+        <v>738157.53510416672</v>
       </c>
       <c r="C21" s="0">
         <v>633.0000065267086</v>
@@ -15587,7 +15587,7 @@
         <v>1</v>
       </c>
       <c r="B22" s="0">
-        <v>737791.53533564811</v>
+        <v>738157.53533564811</v>
       </c>
       <c r="C22" s="0">
         <v>652.99999862909317</v>
@@ -16282,7 +16282,7 @@
         <v>2</v>
       </c>
       <c r="B23" s="0">
-        <v>737791.53571759257</v>
+        <v>738157.53571759257</v>
       </c>
       <c r="C23" s="0">
         <v>686.00000068545341</v>
@@ -16977,7 +16977,7 @@
         <v>2</v>
       </c>
       <c r="B24" s="0">
-        <v>737791.53605324076</v>
+        <v>738157.53605324076</v>
       </c>
       <c r="C24" s="0">
         <v>715.00000432133675</v>
@@ -17672,7 +17672,7 @@
         <v>2</v>
       </c>
       <c r="B25" s="0">
-        <v>737791.53638888884</v>
+        <v>738157.53638888884</v>
       </c>
       <c r="C25" s="0">
         <v>743.99999789893627</v>
@@ -18367,7 +18367,7 @@
         <v>2</v>
       </c>
       <c r="B26" s="0">
-        <v>737791.53673611116</v>
+        <v>738157.53673611116</v>
       </c>
       <c r="C26" s="0">
         <v>774.00000616908073</v>
@@ -19062,7 +19062,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="0">
-        <v>737791.53744212957</v>
+        <v>738157.53744212957</v>
       </c>
       <c r="C27" s="0">
         <v>834.99999716877937</v>
@@ -19757,7 +19757,7 @@
         <v>2</v>
       </c>
       <c r="B28" s="0">
-        <v>737791.53781250003</v>
+        <v>738157.53781250003</v>
       </c>
       <c r="C28" s="0">
         <v>867.00000464916229</v>
@@ -20452,7 +20452,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="0">
-        <v>737791.53811342595</v>
+        <v>738157.53811342595</v>
       </c>
       <c r="C29" s="0">
         <v>893.00000444054604</v>
@@ -21147,7 +21147,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="0">
-        <v>737791.53847222216</v>
+        <v>738157.53847222216</v>
       </c>
       <c r="C30" s="0">
         <v>923.99999722838402</v>
@@ -21842,7 +21842,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="0">
-        <v>737791.53883101849</v>
+        <v>738157.53883101849</v>
       </c>
       <c r="C31" s="0">
         <v>955.00000007450581</v>
@@ -22537,7 +22537,7 @@
         <v>2</v>
       </c>
       <c r="B32" s="0">
-        <v>737791.5391782407</v>
+        <v>738157.5391782407</v>
       </c>
       <c r="C32" s="0">
         <v>984.99999828636646</v>
@@ -23232,7 +23232,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="0">
-        <v>737791.53953703702</v>
+        <v>738157.53953703702</v>
       </c>
       <c r="C33" s="0">
         <v>1016.0000011324883</v>
@@ -23927,7 +23927,7 @@
         <v>2</v>
       </c>
       <c r="B34" s="0">
-        <v>737791.53989583335</v>
+        <v>738157.53989583335</v>
       </c>
       <c r="C34" s="0">
         <v>1047.00000397861</v>
@@ -24622,7 +24622,7 @@
         <v>2</v>
       </c>
       <c r="B35" s="0">
-        <v>737791.54019675928</v>
+        <v>738157.54019675928</v>
       </c>
       <c r="C35" s="0">
         <v>1073.0000037699938</v>
@@ -25317,7 +25317,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="0">
-        <v>737791.54054398148</v>
+        <v>738157.54054398148</v>
       </c>
       <c r="C36" s="0">
         <v>1103.0000019818544</v>
@@ -26012,7 +26012,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="0">
-        <v>737791.54090277781</v>
+        <v>738157.54090277781</v>
       </c>
       <c r="C37" s="0">
         <v>1134.0000048279762</v>
@@ -26707,7 +26707,7 @@
         <v>2</v>
       </c>
       <c r="B38" s="0">
-        <v>737791.54127314815</v>
+        <v>738157.54127314815</v>
       </c>
       <c r="C38" s="0">
         <v>1166.0000022500753</v>
@@ -27402,7 +27402,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="0">
-        <v>737791.54160879634</v>
+        <v>738157.54160879634</v>
       </c>
       <c r="C39" s="0">
         <v>1195.0000058859587</v>
@@ -28097,7 +28097,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="0">
-        <v>737791.54195601854</v>
+        <v>738157.54195601854</v>
       </c>
       <c r="C40" s="0">
         <v>1225.0000040978193</v>

</xml_diff>